<commit_message>
Added full transfer experiments
</commit_message>
<xml_diff>
--- a/experiment_results/final-ant/analysis.xlsx
+++ b/experiment_results/final-ant/analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryedida/Desktop/menzies/dnn-less-data/experiment_results/final-ant/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{747F06A7-F95C-2A45-A597-F4E93768BAA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{962BAC60-DCCB-8042-83CD-0D707036F278}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15900" xr2:uid="{7F1ADA03-CF08-3C48-B918-B6E220B56D2F}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="164">
   <si>
     <t>Our method</t>
   </si>
@@ -475,6 +475,54 @@
   </si>
   <si>
     <t>13.9 (0.4)</t>
+  </si>
+  <si>
+    <t>58.8 (0.0)</t>
+  </si>
+  <si>
+    <t>36.6 (4.6)</t>
+  </si>
+  <si>
+    <t>X12012310</t>
+  </si>
+  <si>
+    <t>4.6 (0.4)</t>
+  </si>
+  <si>
+    <t>5.2 (0.5)</t>
+  </si>
+  <si>
+    <t>28.3 (6.7)</t>
+  </si>
+  <si>
+    <t>41.7 (7.7)</t>
+  </si>
+  <si>
+    <t>52.3 (1.1)</t>
+  </si>
+  <si>
+    <t>19.4 (0.8)</t>
+  </si>
+  <si>
+    <t>19.4 (2.4)</t>
+  </si>
+  <si>
+    <t>32.4 (0.4)</t>
+  </si>
+  <si>
+    <t>28.0 (0.8)</t>
+  </si>
+  <si>
+    <t>48.1 (18.6)</t>
+  </si>
+  <si>
+    <t>77.8 (3.7)</t>
+  </si>
+  <si>
+    <t>12.0 (0.7)</t>
+  </si>
+  <si>
+    <t>11.3 (0.3)</t>
   </si>
 </sst>
 </file>
@@ -992,7 +1040,7 @@
   <dimension ref="A1:S34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1852,14 +1900,33 @@
       <c r="B17" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="11"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="12"/>
-      <c r="K17" s="12"/>
+      <c r="C17" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="D17" s="22" t="s">
+        <v>153</v>
+      </c>
+      <c r="E17" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="F17" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="G17" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="H17" s="22" t="s">
+        <v>154</v>
+      </c>
+      <c r="I17" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="J17" s="22" t="s">
+        <v>148</v>
+      </c>
+      <c r="K17" s="22" t="s">
+        <v>151</v>
+      </c>
       <c r="L17" s="11">
         <v>49</v>
       </c>
@@ -1886,15 +1953,33 @@
       <c r="B18" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="20"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="21"/>
-      <c r="G18" s="20"/>
-      <c r="H18" s="21"/>
-      <c r="I18" s="21"/>
-      <c r="J18" s="21"/>
-      <c r="K18" s="21"/>
+      <c r="C18" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="D18" s="21" t="s">
+        <v>160</v>
+      </c>
+      <c r="E18" s="21" t="s">
+        <v>157</v>
+      </c>
+      <c r="F18" s="21" t="s">
+        <v>158</v>
+      </c>
+      <c r="G18" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="H18" s="21" t="s">
+        <v>163</v>
+      </c>
+      <c r="I18" s="21" t="s">
+        <v>161</v>
+      </c>
+      <c r="J18" s="21" t="s">
+        <v>156</v>
+      </c>
+      <c r="K18" s="21" t="s">
+        <v>159</v>
+      </c>
       <c r="L18" s="20">
         <v>23</v>
       </c>

</xml_diff>